<commit_message>
2019 12 19 1o inclusao de export de agendamento
</commit_message>
<xml_diff>
--- a/testemunhoweb/logs/November.xlsx
+++ b/testemunhoweb/logs/November.xlsx
@@ -451,57 +451,19 @@
       <c r="M2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Sexta-feira</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>Keila</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>Isabele</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr"/>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t>Aline Melo</t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>Valquiria</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="inlineStr"/>
-      <c r="I3" s="4" t="inlineStr"/>
-      <c r="J3" s="4" t="inlineStr">
-        <is>
-          <t>Aline Lima</t>
-        </is>
-      </c>
-      <c r="K3" s="4" t="inlineStr">
-        <is>
-          <t>Beth</t>
-        </is>
-      </c>
-      <c r="L3" s="4" t="inlineStr">
-        <is>
-          <t>Rodolfo Dias</t>
-        </is>
-      </c>
-      <c r="M3" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
-        </is>
-      </c>
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="4" t="n"/>
+      <c r="D3" s="4" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="4" t="n"/>
+      <c r="I3" s="4" t="n"/>
+      <c r="J3" s="4" t="n"/>
+      <c r="K3" s="4" t="n"/>
+      <c r="L3" s="4" t="n"/>
+      <c r="M3" s="4" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
@@ -509,51 +471,97 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Sabado</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr"/>
-      <c r="D4" s="4" t="inlineStr"/>
+          <t>Segunda-feira</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>EMPTY</t>
+        </is>
+      </c>
       <c r="E4" s="4" t="inlineStr"/>
-      <c r="F4" s="4" t="inlineStr"/>
-      <c r="G4" s="4" t="inlineStr"/>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Alana</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
       <c r="H4" s="4" t="inlineStr"/>
       <c r="I4" s="4" t="inlineStr"/>
       <c r="J4" s="4" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Vinicius</t>
         </is>
       </c>
       <c r="K4" s="4" t="inlineStr">
         <is>
-          <t>Telma</t>
+          <t>Icaro</t>
         </is>
       </c>
       <c r="L4" s="4" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="M4" s="4" t="inlineStr">
         <is>
-          <t>Geronimo</t>
+          <t>EMPTY</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n"/>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="4" t="n"/>
-      <c r="D5" s="4" t="n"/>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="n"/>
-      <c r="H5" s="4" t="n"/>
-      <c r="I5" s="4" t="n"/>
-      <c r="J5" s="4" t="n"/>
-      <c r="K5" s="4" t="n"/>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="4" t="n"/>
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Terca-feira</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>Lindoia</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Cida</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr"/>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>Luciana</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Valquiria</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr"/>
+      <c r="I5" s="4" t="inlineStr"/>
+      <c r="J5" s="4" t="inlineStr">
+        <is>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>Alana</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="inlineStr"/>
+      <c r="M5" s="4" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
@@ -561,52 +569,44 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Segunda-feira</t>
+          <t>Quarta-feira</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Ediane</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr"/>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Robson</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr"/>
       <c r="I6" s="4" t="inlineStr"/>
       <c r="J6" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="K6" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
-        </is>
-      </c>
-      <c r="L6" s="4" t="inlineStr">
-        <is>
-          <t>Marcio</t>
-        </is>
-      </c>
-      <c r="M6" s="4" t="inlineStr">
-        <is>
-          <t>Amintas</t>
-        </is>
-      </c>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="inlineStr"/>
+      <c r="M6" s="4" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
@@ -614,42 +614,26 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Terca-feira</t>
+          <t>Quinta-feira</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Marileia</t>
         </is>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
+          <t>Helaine Camilo</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr"/>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Luciana</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>Valquiria</t>
-        </is>
-      </c>
+      <c r="F7" s="4" t="inlineStr"/>
+      <c r="G7" s="4" t="inlineStr"/>
       <c r="H7" s="4" t="inlineStr"/>
       <c r="I7" s="4" t="inlineStr"/>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>Lucia</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>Daiana</t>
-        </is>
-      </c>
+      <c r="J7" s="4" t="inlineStr"/>
+      <c r="K7" s="4" t="inlineStr"/>
       <c r="L7" s="4" t="inlineStr"/>
       <c r="M7" s="4" t="inlineStr"/>
     </row>
@@ -659,44 +643,52 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Quarta-feira</t>
+          <t>Sexta-feira</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr"/>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Aline Melo</t>
         </is>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>Conceicao</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr"/>
       <c r="I8" s="4" t="inlineStr"/>
       <c r="J8" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Aline Lima</t>
         </is>
       </c>
       <c r="K8" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L8" s="4" t="inlineStr"/>
-      <c r="M8" s="4" t="inlineStr"/>
+          <t>Beth</t>
+        </is>
+      </c>
+      <c r="L8" s="4" t="inlineStr">
+        <is>
+          <t>Clayton</t>
+        </is>
+      </c>
+      <c r="M8" s="4" t="inlineStr">
+        <is>
+          <t>Rodolfo</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="n">
@@ -704,81 +696,51 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Quinta-feira</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>Marileia</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
-        </is>
-      </c>
+          <t>Sabado</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr"/>
+      <c r="D9" s="4" t="inlineStr"/>
       <c r="E9" s="4" t="inlineStr"/>
       <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" s="4" t="inlineStr"/>
       <c r="H9" s="4" t="inlineStr"/>
       <c r="I9" s="4" t="inlineStr"/>
-      <c r="J9" s="4" t="inlineStr"/>
-      <c r="K9" s="4" t="inlineStr"/>
-      <c r="L9" s="4" t="inlineStr"/>
-      <c r="M9" s="4" t="inlineStr"/>
+      <c r="J9" s="4" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="K9" s="4" t="inlineStr">
+        <is>
+          <t>Davi</t>
+        </is>
+      </c>
+      <c r="L9" s="4" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="M9" s="4" t="inlineStr">
+        <is>
+          <t>Icaro</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>Sexta-feira</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>Edith</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="inlineStr">
-        <is>
-          <t>Daiana</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr"/>
-      <c r="F10" s="4" t="inlineStr">
-        <is>
-          <t>Aline Melo</t>
-        </is>
-      </c>
-      <c r="G10" s="4" t="inlineStr">
-        <is>
-          <t>Antonio</t>
-        </is>
-      </c>
-      <c r="H10" s="4" t="inlineStr"/>
-      <c r="I10" s="4" t="inlineStr"/>
-      <c r="J10" s="4" t="inlineStr">
-        <is>
-          <t>Lucia</t>
-        </is>
-      </c>
-      <c r="K10" s="4" t="inlineStr">
-        <is>
-          <t>Lurdes</t>
-        </is>
-      </c>
-      <c r="L10" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
-        </is>
-      </c>
-      <c r="M10" s="4" t="inlineStr">
-        <is>
-          <t>Clayton</t>
-        </is>
-      </c>
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="4" t="n"/>
+      <c r="E10" s="4" t="n"/>
+      <c r="F10" s="4" t="n"/>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="4" t="n"/>
+      <c r="I10" s="4" t="n"/>
+      <c r="J10" s="4" t="n"/>
+      <c r="K10" s="4" t="n"/>
+      <c r="L10" s="4" t="n"/>
+      <c r="M10" s="4" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="3" t="n">
@@ -786,51 +748,97 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Sabado</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr"/>
-      <c r="D11" s="4" t="inlineStr"/>
+          <t>Segunda-feira</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>Lurdes</t>
+        </is>
+      </c>
       <c r="E11" s="4" t="inlineStr"/>
-      <c r="F11" s="4" t="inlineStr"/>
-      <c r="G11" s="4" t="inlineStr"/>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>Graca</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>EMPTY</t>
+        </is>
+      </c>
       <c r="H11" s="4" t="inlineStr"/>
       <c r="I11" s="4" t="inlineStr"/>
       <c r="J11" s="4" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K11" s="4" t="inlineStr">
         <is>
-          <t>Karol</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Amintas</t>
         </is>
       </c>
       <c r="M11" s="4" t="inlineStr">
         <is>
-          <t>Douglas Oliveira</t>
+          <t>Antonio</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="4" t="n"/>
-      <c r="D12" s="4" t="n"/>
-      <c r="E12" s="4" t="n"/>
-      <c r="F12" s="4" t="n"/>
-      <c r="G12" s="4" t="n"/>
-      <c r="H12" s="4" t="n"/>
-      <c r="I12" s="4" t="n"/>
-      <c r="J12" s="4" t="n"/>
-      <c r="K12" s="4" t="n"/>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="4" t="n"/>
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Terca-feira</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>Lindoia</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>Graca</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr"/>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Luciana</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Patricia Rodrigues</t>
+        </is>
+      </c>
+      <c r="H12" s="4" t="inlineStr"/>
+      <c r="I12" s="4" t="inlineStr"/>
+      <c r="J12" s="4" t="inlineStr">
+        <is>
+          <t>Icaro</t>
+        </is>
+      </c>
+      <c r="K12" s="4" t="inlineStr">
+        <is>
+          <t>Rodolfo</t>
+        </is>
+      </c>
+      <c r="L12" s="4" t="inlineStr"/>
+      <c r="M12" s="4" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="3" t="n">
@@ -838,28 +846,28 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Segunda-feira</t>
+          <t>Quarta-feira</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Ediane</t>
         </is>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr"/>
       <c r="F13" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Conceicao</t>
         </is>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="H13" s="4" t="inlineStr"/>
@@ -871,19 +879,11 @@
       </c>
       <c r="K13" s="4" t="inlineStr">
         <is>
-          <t>Icaro</t>
-        </is>
-      </c>
-      <c r="L13" s="4" t="inlineStr">
-        <is>
-          <t>Vanda</t>
-        </is>
-      </c>
-      <c r="M13" s="4" t="inlineStr">
-        <is>
           <t>EMPTY</t>
         </is>
       </c>
+      <c r="L13" s="4" t="inlineStr"/>
+      <c r="M13" s="4" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="n">
@@ -891,42 +891,26 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Terca-feira</t>
+          <t>Quinta-feira</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
+          <t>Marileia</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
           <t>Lindoia</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr">
-        <is>
-          <t>Eliane</t>
-        </is>
-      </c>
       <c r="E14" s="4" t="inlineStr"/>
-      <c r="F14" s="4" t="inlineStr">
-        <is>
-          <t>Luciana</t>
-        </is>
-      </c>
-      <c r="G14" s="4" t="inlineStr">
-        <is>
-          <t>Patricia Rodrigues</t>
-        </is>
-      </c>
+      <c r="F14" s="4" t="inlineStr"/>
+      <c r="G14" s="4" t="inlineStr"/>
       <c r="H14" s="4" t="inlineStr"/>
       <c r="I14" s="4" t="inlineStr"/>
-      <c r="J14" s="4" t="inlineStr">
-        <is>
-          <t>Jessica Silva</t>
-        </is>
-      </c>
-      <c r="K14" s="4" t="inlineStr">
-        <is>
-          <t>Alana</t>
-        </is>
-      </c>
+      <c r="J14" s="4" t="inlineStr"/>
+      <c r="K14" s="4" t="inlineStr"/>
       <c r="L14" s="4" t="inlineStr"/>
       <c r="M14" s="4" t="inlineStr"/>
     </row>
@@ -936,44 +920,52 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Quarta-feira</t>
+          <t>Sexta-feira</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Isabele</t>
         </is>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr"/>
       <c r="F15" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Aline Melo</t>
         </is>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>Robson</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H15" s="4" t="inlineStr"/>
       <c r="I15" s="4" t="inlineStr"/>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Daiana</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L15" s="4" t="inlineStr"/>
-      <c r="M15" s="4" t="inlineStr"/>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="L15" s="4" t="inlineStr">
+        <is>
+          <t>Icaro</t>
+        </is>
+      </c>
+      <c r="M15" s="4" t="inlineStr">
+        <is>
+          <t>Vinicius</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="n">
@@ -981,81 +973,51 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Quinta-feira</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>Marileia</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
+          <t>Sabado</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr"/>
+      <c r="D16" s="4" t="inlineStr"/>
       <c r="E16" s="4" t="inlineStr"/>
       <c r="F16" s="4" t="inlineStr"/>
       <c r="G16" s="4" t="inlineStr"/>
       <c r="H16" s="4" t="inlineStr"/>
       <c r="I16" s="4" t="inlineStr"/>
-      <c r="J16" s="4" t="inlineStr"/>
-      <c r="K16" s="4" t="inlineStr"/>
-      <c r="L16" s="4" t="inlineStr"/>
-      <c r="M16" s="4" t="inlineStr"/>
+      <c r="J16" s="4" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="K16" s="4" t="inlineStr">
+        <is>
+          <t>Beth</t>
+        </is>
+      </c>
+      <c r="L16" s="4" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="M16" s="4" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="inlineStr">
-        <is>
-          <t>Sexta-feira</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>Keila</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="inlineStr">
-        <is>
-          <t>Isabele</t>
-        </is>
-      </c>
-      <c r="E17" s="4" t="inlineStr"/>
-      <c r="F17" s="4" t="inlineStr">
-        <is>
-          <t>Aline Melo</t>
-        </is>
-      </c>
-      <c r="G17" s="4" t="inlineStr">
-        <is>
-          <t>Valquiria</t>
-        </is>
-      </c>
-      <c r="H17" s="4" t="inlineStr"/>
-      <c r="I17" s="4" t="inlineStr"/>
-      <c r="J17" s="4" t="inlineStr">
-        <is>
-          <t>Aline Lima</t>
-        </is>
-      </c>
-      <c r="K17" s="4" t="inlineStr">
-        <is>
-          <t>Beth</t>
-        </is>
-      </c>
-      <c r="L17" s="4" t="inlineStr">
-        <is>
-          <t>Rodolfo Dias</t>
-        </is>
-      </c>
-      <c r="M17" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
-        </is>
-      </c>
+      <c r="A17" s="3" t="n"/>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="4" t="n"/>
+      <c r="D17" s="4" t="n"/>
+      <c r="E17" s="4" t="n"/>
+      <c r="F17" s="4" t="n"/>
+      <c r="G17" s="4" t="n"/>
+      <c r="H17" s="4" t="n"/>
+      <c r="I17" s="4" t="n"/>
+      <c r="J17" s="4" t="n"/>
+      <c r="K17" s="4" t="n"/>
+      <c r="L17" s="4" t="n"/>
+      <c r="M17" s="4" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="n">
@@ -1063,51 +1025,97 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Sabado</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="inlineStr"/>
-      <c r="D18" s="4" t="inlineStr"/>
+          <t>Segunda-feira</t>
+        </is>
+      </c>
+      <c r="C18" s="4" t="inlineStr">
+        <is>
+          <t>Helaine Camilo</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
       <c r="E18" s="4" t="inlineStr"/>
-      <c r="F18" s="4" t="inlineStr"/>
-      <c r="G18" s="4" t="inlineStr"/>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Alana</t>
+        </is>
+      </c>
       <c r="H18" s="4" t="inlineStr"/>
       <c r="I18" s="4" t="inlineStr"/>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>Davi</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="L18" s="4" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Marcio</t>
         </is>
       </c>
       <c r="M18" s="4" t="inlineStr">
         <is>
-          <t>Geronimo</t>
+          <t>Icaro</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n"/>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="4" t="n"/>
-      <c r="D19" s="4" t="n"/>
-      <c r="E19" s="4" t="n"/>
-      <c r="F19" s="4" t="n"/>
-      <c r="G19" s="4" t="n"/>
-      <c r="H19" s="4" t="n"/>
-      <c r="I19" s="4" t="n"/>
-      <c r="J19" s="4" t="n"/>
-      <c r="K19" s="4" t="n"/>
-      <c r="L19" s="4" t="n"/>
-      <c r="M19" s="4" t="n"/>
+      <c r="A19" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Terca-feira</t>
+        </is>
+      </c>
+      <c r="C19" s="4" t="inlineStr">
+        <is>
+          <t>Lindoia</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>Daiana</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr"/>
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Luciana</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Valquiria</t>
+        </is>
+      </c>
+      <c r="H19" s="4" t="inlineStr"/>
+      <c r="I19" s="4" t="inlineStr"/>
+      <c r="J19" s="4" t="inlineStr">
+        <is>
+          <t>Jessica Silva</t>
+        </is>
+      </c>
+      <c r="K19" s="4" t="inlineStr">
+        <is>
+          <t>Keila</t>
+        </is>
+      </c>
+      <c r="L19" s="4" t="inlineStr"/>
+      <c r="M19" s="4" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="n">
@@ -1115,52 +1123,44 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Segunda-feira</t>
+          <t>Quarta-feira</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Ediane</t>
         </is>
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr"/>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>Graca</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>Aline Lima</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr"/>
       <c r="I20" s="4" t="inlineStr"/>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>Keila</t>
-        </is>
-      </c>
-      <c r="L20" s="4" t="inlineStr">
-        <is>
-          <t>Amintas</t>
-        </is>
-      </c>
-      <c r="M20" s="4" t="inlineStr">
-        <is>
-          <t>Dario</t>
-        </is>
-      </c>
+          <t>Lurdes</t>
+        </is>
+      </c>
+      <c r="L20" s="4" t="inlineStr"/>
+      <c r="M20" s="4" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
@@ -1168,42 +1168,26 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Terca-feira</t>
+          <t>Quinta-feira</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Marileia</t>
         </is>
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>Cida</t>
+          <t>Alana</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr"/>
-      <c r="F21" s="4" t="inlineStr">
-        <is>
-          <t>Luciana</t>
-        </is>
-      </c>
-      <c r="G21" s="4" t="inlineStr">
-        <is>
-          <t>Daiana</t>
-        </is>
-      </c>
+      <c r="F21" s="4" t="inlineStr"/>
+      <c r="G21" s="4" t="inlineStr"/>
       <c r="H21" s="4" t="inlineStr"/>
       <c r="I21" s="4" t="inlineStr"/>
-      <c r="J21" s="4" t="inlineStr">
-        <is>
-          <t>Rodolfo Dias</t>
-        </is>
-      </c>
-      <c r="K21" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
-        </is>
-      </c>
+      <c r="J21" s="4" t="inlineStr"/>
+      <c r="K21" s="4" t="inlineStr"/>
       <c r="L21" s="4" t="inlineStr"/>
       <c r="M21" s="4" t="inlineStr"/>
     </row>
@@ -1213,44 +1197,52 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Quarta-feira</t>
+          <t>Sexta-feira</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>Lurdes</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr"/>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>Valquiria</t>
+          <t>Aline Melo</t>
         </is>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="H22" s="4" t="inlineStr"/>
       <c r="I22" s="4" t="inlineStr"/>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
+          <t>Beth</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr"/>
-      <c r="M22" s="4" t="inlineStr"/>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
+        <is>
+          <t>Clayton</t>
+        </is>
+      </c>
+      <c r="M22" s="4" t="inlineStr">
+        <is>
+          <t>Rodolfo</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
@@ -1258,81 +1250,51 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Quinta-feira</t>
-        </is>
-      </c>
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>Marileia</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="inlineStr">
-        <is>
-          <t>Lurdes</t>
-        </is>
-      </c>
+          <t>Sabado</t>
+        </is>
+      </c>
+      <c r="C23" s="4" t="inlineStr"/>
+      <c r="D23" s="4" t="inlineStr"/>
       <c r="E23" s="4" t="inlineStr"/>
       <c r="F23" s="4" t="inlineStr"/>
       <c r="G23" s="4" t="inlineStr"/>
       <c r="H23" s="4" t="inlineStr"/>
       <c r="I23" s="4" t="inlineStr"/>
-      <c r="J23" s="4" t="inlineStr"/>
-      <c r="K23" s="4" t="inlineStr"/>
-      <c r="L23" s="4" t="inlineStr"/>
-      <c r="M23" s="4" t="inlineStr"/>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo</t>
+        </is>
+      </c>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="M23" s="4" t="inlineStr">
+        <is>
+          <t>Eliane</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" s="3" t="inlineStr">
-        <is>
-          <t>Sexta-feira</t>
-        </is>
-      </c>
-      <c r="C24" s="4" t="inlineStr">
-        <is>
-          <t>Lurdes</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="inlineStr">
-        <is>
-          <t>Eliane</t>
-        </is>
-      </c>
-      <c r="E24" s="4" t="inlineStr"/>
-      <c r="F24" s="4" t="inlineStr">
-        <is>
-          <t>Aline Melo</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>Patricia Rodrigues</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr"/>
-      <c r="I24" s="4" t="inlineStr"/>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>Antonio</t>
-        </is>
-      </c>
-      <c r="K24" s="4" t="inlineStr">
-        <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L24" s="4" t="inlineStr">
-        <is>
-          <t>Clayton</t>
-        </is>
-      </c>
-      <c r="M24" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
-        </is>
-      </c>
+      <c r="A24" s="3" t="n"/>
+      <c r="B24" s="3" t="n"/>
+      <c r="C24" s="4" t="n"/>
+      <c r="D24" s="4" t="n"/>
+      <c r="E24" s="4" t="n"/>
+      <c r="F24" s="4" t="n"/>
+      <c r="G24" s="4" t="n"/>
+      <c r="H24" s="4" t="n"/>
+      <c r="I24" s="4" t="n"/>
+      <c r="J24" s="4" t="n"/>
+      <c r="K24" s="4" t="n"/>
+      <c r="L24" s="4" t="n"/>
+      <c r="M24" s="4" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
@@ -1340,51 +1302,97 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Sabado</t>
-        </is>
-      </c>
-      <c r="C25" s="4" t="inlineStr"/>
-      <c r="D25" s="4" t="inlineStr"/>
+          <t>Segunda-feira</t>
+        </is>
+      </c>
+      <c r="C25" s="4" t="inlineStr">
+        <is>
+          <t>Lucia</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="inlineStr">
+        <is>
+          <t>Lurdes</t>
+        </is>
+      </c>
       <c r="E25" s="4" t="inlineStr"/>
-      <c r="F25" s="4" t="inlineStr"/>
-      <c r="G25" s="4" t="inlineStr"/>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>Graca</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>EMPTY</t>
+        </is>
+      </c>
       <c r="H25" s="4" t="inlineStr"/>
       <c r="I25" s="4" t="inlineStr"/>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
         <is>
-          <t>Telma</t>
+          <t>Eliane</t>
         </is>
       </c>
       <c r="L25" s="4" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Amintas</t>
         </is>
       </c>
       <c r="M25" s="4" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Dario</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n"/>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
+      <c r="A26" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Terca-feira</t>
+        </is>
+      </c>
+      <c r="C26" s="4" t="inlineStr">
+        <is>
+          <t>Lindoia</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="inlineStr">
+        <is>
+          <t>Edith</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr"/>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Luciana</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Rodolfo</t>
+        </is>
+      </c>
+      <c r="H26" s="4" t="inlineStr"/>
+      <c r="I26" s="4" t="inlineStr"/>
+      <c r="J26" s="4" t="inlineStr">
+        <is>
+          <t>Icaro</t>
+        </is>
+      </c>
+      <c r="K26" s="4" t="inlineStr">
+        <is>
+          <t>EMPTY</t>
+        </is>
+      </c>
+      <c r="L26" s="4" t="inlineStr"/>
+      <c r="M26" s="4" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
@@ -1392,52 +1400,44 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Segunda-feira</t>
+          <t>Quarta-feira</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Helaine Camilo</t>
+          <t>Rodolfo</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>Alana</t>
+          <t>Lindoia</t>
         </is>
       </c>
       <c r="E27" s="4" t="inlineStr"/>
       <c r="F27" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>EMPTY</t>
+          <t>Robson</t>
         </is>
       </c>
       <c r="H27" s="4" t="inlineStr"/>
       <c r="I27" s="4" t="inlineStr"/>
       <c r="J27" s="4" t="inlineStr">
         <is>
-          <t>Vinicius</t>
+          <t>Antonio</t>
         </is>
       </c>
       <c r="K27" s="4" t="inlineStr">
         <is>
-          <t>Antonio</t>
-        </is>
-      </c>
-      <c r="L27" s="4" t="inlineStr">
-        <is>
-          <t>Marcio</t>
-        </is>
-      </c>
-      <c r="M27" s="4" t="inlineStr">
-        <is>
-          <t>Icaro</t>
-        </is>
-      </c>
+          <t>EMPTY</t>
+        </is>
+      </c>
+      <c r="L27" s="4" t="inlineStr"/>
+      <c r="M27" s="4" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
@@ -1445,42 +1445,26 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Terca-feira</t>
+          <t>Quinta-feira</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Marileia</t>
         </is>
       </c>
       <c r="D28" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Keila</t>
         </is>
       </c>
       <c r="E28" s="4" t="inlineStr"/>
-      <c r="F28" s="4" t="inlineStr">
-        <is>
-          <t>Luciana</t>
-        </is>
-      </c>
-      <c r="G28" s="4" t="inlineStr">
-        <is>
-          <t>Patricia Rodrigues</t>
-        </is>
-      </c>
+      <c r="F28" s="4" t="inlineStr"/>
+      <c r="G28" s="4" t="inlineStr"/>
       <c r="H28" s="4" t="inlineStr"/>
       <c r="I28" s="4" t="inlineStr"/>
-      <c r="J28" s="4" t="inlineStr">
-        <is>
-          <t>Alana</t>
-        </is>
-      </c>
-      <c r="K28" s="4" t="inlineStr">
-        <is>
-          <t>Keila</t>
-        </is>
-      </c>
+      <c r="J28" s="4" t="inlineStr"/>
+      <c r="K28" s="4" t="inlineStr"/>
       <c r="L28" s="4" t="inlineStr"/>
       <c r="M28" s="4" t="inlineStr"/>
     </row>
@@ -1490,44 +1474,52 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Quarta-feira</t>
+          <t>Sexta-feira</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Rodolfo Dias</t>
+          <t>Lurdes</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>Lindoia</t>
+          <t>Isabele</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr"/>
       <c r="F29" s="4" t="inlineStr">
         <is>
-          <t>Patricia Dias</t>
+          <t>Aline Melo</t>
         </is>
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>Robson</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="H29" s="4" t="inlineStr"/>
       <c r="I29" s="4" t="inlineStr"/>
       <c r="J29" s="4" t="inlineStr">
         <is>
-          <t>Vanda</t>
+          <t>Lucia</t>
         </is>
       </c>
       <c r="K29" s="4" t="inlineStr">
         <is>
+          <t>Daiana</t>
+        </is>
+      </c>
+      <c r="L29" s="4" t="inlineStr">
+        <is>
+          <t>Vinicius</t>
+        </is>
+      </c>
+      <c r="M29" s="4" t="inlineStr">
+        <is>
           <t>EMPTY</t>
         </is>
       </c>
-      <c r="L29" s="4" t="inlineStr"/>
-      <c r="M29" s="4" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
@@ -1535,81 +1527,51 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Quinta-feira</t>
-        </is>
-      </c>
-      <c r="C30" s="4" t="inlineStr">
-        <is>
-          <t>Marileia</t>
-        </is>
-      </c>
-      <c r="D30" s="4" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
+          <t>Sabado</t>
+        </is>
+      </c>
+      <c r="C30" s="4" t="inlineStr"/>
+      <c r="D30" s="4" t="inlineStr"/>
       <c r="E30" s="4" t="inlineStr"/>
       <c r="F30" s="4" t="inlineStr"/>
       <c r="G30" s="4" t="inlineStr"/>
       <c r="H30" s="4" t="inlineStr"/>
       <c r="I30" s="4" t="inlineStr"/>
-      <c r="J30" s="4" t="inlineStr"/>
-      <c r="K30" s="4" t="inlineStr"/>
-      <c r="L30" s="4" t="inlineStr"/>
-      <c r="M30" s="4" t="inlineStr"/>
+      <c r="J30" s="4" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="K30" s="4" t="inlineStr">
+        <is>
+          <t>Beth</t>
+        </is>
+      </c>
+      <c r="L30" s="4" t="inlineStr">
+        <is>
+          <t>Samuel</t>
+        </is>
+      </c>
+      <c r="M30" s="4" t="inlineStr">
+        <is>
+          <t>Douglas Oliveira</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" s="3" t="inlineStr">
-        <is>
-          <t>Sexta-feira</t>
-        </is>
-      </c>
-      <c r="C31" s="4" t="inlineStr">
-        <is>
-          <t>Daiana</t>
-        </is>
-      </c>
-      <c r="D31" s="4" t="inlineStr">
-        <is>
-          <t>Isabele</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="inlineStr"/>
-      <c r="F31" s="4" t="inlineStr">
-        <is>
-          <t>Aline Melo</t>
-        </is>
-      </c>
-      <c r="G31" s="4" t="inlineStr">
-        <is>
-          <t>Lucia</t>
-        </is>
-      </c>
-      <c r="H31" s="4" t="inlineStr"/>
-      <c r="I31" s="4" t="inlineStr"/>
-      <c r="J31" s="4" t="inlineStr">
-        <is>
-          <t>Vinicius</t>
-        </is>
-      </c>
-      <c r="K31" s="4" t="inlineStr">
-        <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
-      <c r="L31" s="4" t="inlineStr">
-        <is>
-          <t>Rodolfo Dias</t>
-        </is>
-      </c>
-      <c r="M31" s="4" t="inlineStr">
-        <is>
-          <t>EMPTY</t>
-        </is>
-      </c>
+      <c r="A31" s="3" t="n"/>
+      <c r="B31" s="3" t="n"/>
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="4" t="n"/>
+      <c r="E31" s="4" t="n"/>
+      <c r="F31" s="4" t="n"/>
+      <c r="G31" s="4" t="n"/>
+      <c r="H31" s="4" t="n"/>
+      <c r="I31" s="4" t="n"/>
+      <c r="J31" s="4" t="n"/>
+      <c r="K31" s="4" t="n"/>
+      <c r="L31" s="4" t="n"/>
+      <c r="M31" s="4" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="n">
@@ -1617,34 +1579,50 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Sabado</t>
-        </is>
-      </c>
-      <c r="C32" s="4" t="inlineStr"/>
-      <c r="D32" s="4" t="inlineStr"/>
+          <t>Segunda-feira</t>
+        </is>
+      </c>
+      <c r="C32" s="4" t="inlineStr">
+        <is>
+          <t>Alana</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr">
+        <is>
+          <t>Helaine Camilo</t>
+        </is>
+      </c>
       <c r="E32" s="4" t="inlineStr"/>
-      <c r="F32" s="4" t="inlineStr"/>
-      <c r="G32" s="4" t="inlineStr"/>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>Aline Lima</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>EMPTY</t>
+        </is>
+      </c>
       <c r="H32" s="4" t="inlineStr"/>
       <c r="I32" s="4" t="inlineStr"/>
       <c r="J32" s="4" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Patricia Dias</t>
         </is>
       </c>
       <c r="K32" s="4" t="inlineStr">
         <is>
-          <t>Davi</t>
+          <t>Valquiria</t>
         </is>
       </c>
       <c r="L32" s="4" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Vanda</t>
         </is>
       </c>
       <c r="M32" s="4" t="inlineStr">
         <is>
-          <t>Eliane</t>
+          <t>EMPTY</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1649,7 @@
       </c>
       <c r="B34" s="3" t="n"/>
       <c r="C34" s="5" t="n">
-        <v>43805.00961536479</v>
+        <v>43819.03027682129</v>
       </c>
       <c r="D34" s="4" t="n"/>
       <c r="E34" s="4" t="n"/>

</xml_diff>